<commit_message>
Adding brainstorming ideas for calculations
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C1B086-FB06-4C5A-A3E0-E31B040CD13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672DEA63-CC2C-48EF-9C6B-06D596721BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="169">
   <si>
     <t>table_name</t>
   </si>
@@ -322,9 +322,6 @@
     <t xml:space="preserve">N </t>
   </si>
   <si>
-    <t>customer_name</t>
-  </si>
-  <si>
     <t>customer_city</t>
   </si>
   <si>
@@ -416,6 +413,135 @@
   </si>
   <si>
     <t>territory</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Count of categoryname bringing in the most revenue</t>
+  </si>
+  <si>
+    <t>count of customer who oders the most</t>
+  </si>
+  <si>
+    <t>customer contact who has the most leadership position or lowest position in the company</t>
+  </si>
+  <si>
+    <t>leadship position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate the region where most or least amount of northwind customers are located </t>
+  </si>
+  <si>
+    <t>calculate city where most or least amount of northwind customers are located</t>
+  </si>
+  <si>
+    <t>calculate the postalcode where most or least amountof northwind customers are located</t>
+  </si>
+  <si>
+    <t>calculate the country where most or least amount of northwind customers are located</t>
+  </si>
+  <si>
+    <t>calculate hight performance or employee that manages the most orders/customers</t>
+  </si>
+  <si>
+    <t>calculate the employees highest leadership postion or the lowest position in the company</t>
+  </si>
+  <si>
+    <t>calculate the amount of employees who could be marries single or have a doctor's degree</t>
+  </si>
+  <si>
+    <t>calculate the employees age</t>
+  </si>
+  <si>
+    <t>calculate how long the employees have been in the company</t>
+  </si>
+  <si>
+    <t>calculate the city where most of our employees are located vs where the least amount of employees reside</t>
+  </si>
+  <si>
+    <t>calculate the postalcode where most or least amountof northwind employees are located</t>
+  </si>
+  <si>
+    <t>calculate the country where most or least amount of northwind employees are located</t>
+  </si>
+  <si>
+    <t>help me calculate the highest leadership position or the lowest position in the company depending on the amount of employees reporting to a particular person</t>
+  </si>
+  <si>
+    <t>calculate with employee name which territory most or lowest amount of employees are located</t>
+  </si>
+  <si>
+    <t>calculate the revenue of each product sold by the amount order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glancing at the data there are no discount values in this column but I would have calculated the revenue after discount amount </t>
+  </si>
+  <si>
+    <t>calculate the most frequent shipper used</t>
+  </si>
+  <si>
+    <t>calculate the cost of the freight ordered and see how mean, max, and lowest amount customer spends</t>
+  </si>
+  <si>
+    <t>Use this column to calculate how much each customer spends per order</t>
+  </si>
+  <si>
+    <t>calculate the region where most or least amount of  items are shipping to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate the postalcode where most or least amount of  items are shipping to </t>
+  </si>
+  <si>
+    <t>calculate the most frequent city or least frequent city where items are shipping to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate the country where most or least amount of items are shipping to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can use this column to calculate the most demanded product </t>
+  </si>
+  <si>
+    <t>calculate which supplier produces the most or least amount of items</t>
+  </si>
+  <si>
+    <t>calculate which category is the highest seller/ more in demand</t>
+  </si>
+  <si>
+    <t>calculate how much product we would need to have in stock</t>
+  </si>
+  <si>
+    <t>calculate the amount of all products that we have in stock, on order, and on reorder to view our spending</t>
+  </si>
+  <si>
+    <t>calculate the amount of all products that have been discountinued and no longer have those products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate the region where most or least amount of territories fall under </t>
+  </si>
+  <si>
+    <t>calculate the most used shipper that takes the product to the customer</t>
+  </si>
+  <si>
+    <t>calculate the supplier that produces most or least of the products</t>
+  </si>
+  <si>
+    <t>calculate the highest leadership position of the contact name based on title</t>
+  </si>
+  <si>
+    <t>calculate the city where most or least amount of suppliers are located</t>
+  </si>
+  <si>
+    <t>calculate the region where most or least amount of suppliers are located</t>
+  </si>
+  <si>
+    <t>calculate the postcode where most or least amount of suppliers are located</t>
+  </si>
+  <si>
+    <t>calculate the postalcode where emost or least amount of suppliers are located</t>
+  </si>
+  <si>
+    <t>calculate most or least amount of territories are in the region</t>
   </si>
 </sst>
 </file>
@@ -803,11 +929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B56A5E-AA28-4DB9-BAE3-51DE131C631E}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K61" sqref="K61"/>
+      <selection pane="bottomRight" activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,8 +948,9 @@
     <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="133.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -898,6 +1025,18 @@
       <c r="I2" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -927,6 +1066,18 @@
       <c r="I3" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -956,6 +1107,18 @@
       <c r="I4" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -985,6 +1148,18 @@
       <c r="I5" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1014,6 +1189,18 @@
       <c r="I6" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1041,7 +1228,19 @@
         <v>91</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1070,7 +1269,19 @@
         <v>91</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1096,10 +1307,22 @@
         <v>92</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1130,6 +1353,18 @@
       <c r="I10" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1157,7 +1392,19 @@
         <v>91</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1186,7 +1433,19 @@
         <v>91</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -1215,7 +1474,19 @@
         <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1244,7 +1515,19 @@
         <v>91</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1275,6 +1558,18 @@
       <c r="I15" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="J15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1304,8 +1599,20 @@
       <c r="I16" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1333,8 +1640,20 @@
       <c r="I17" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1360,10 +1679,22 @@
         <v>91</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1389,10 +1720,22 @@
         <v>91</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1418,10 +1761,22 @@
         <v>91</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1447,10 +1802,22 @@
         <v>91</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1476,10 +1843,22 @@
         <v>91</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1505,10 +1884,22 @@
         <v>91</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1536,8 +1927,20 @@
       <c r="I24" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1563,10 +1966,22 @@
         <v>91</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1592,10 +2007,22 @@
         <v>91</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1621,10 +2048,22 @@
         <v>91</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1650,10 +2089,22 @@
         <v>92</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1681,8 +2132,20 @@
       <c r="I29" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1710,8 +2173,20 @@
       <c r="I30" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1739,8 +2214,20 @@
       <c r="I31" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1768,8 +2255,20 @@
       <c r="I32" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1797,8 +2296,20 @@
       <c r="I33" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
@@ -1826,8 +2337,20 @@
       <c r="I34" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -1855,8 +2378,20 @@
       <c r="I35" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -1884,8 +2419,20 @@
       <c r="I36" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1913,8 +2460,20 @@
       <c r="I37" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1942,8 +2501,20 @@
       <c r="I38" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1969,10 +2540,22 @@
         <v>91</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -2000,8 +2583,20 @@
       <c r="I40" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
@@ -2029,8 +2624,20 @@
       <c r="I41" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
@@ -2058,8 +2665,20 @@
       <c r="I42" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -2087,8 +2706,20 @@
       <c r="I43" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -2116,8 +2747,20 @@
       <c r="I44" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>53</v>
       </c>
@@ -2145,8 +2788,20 @@
       <c r="I45" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -2174,8 +2829,20 @@
       <c r="I46" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -2203,8 +2870,20 @@
       <c r="I47" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
@@ -2230,10 +2909,22 @@
         <v>91</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -2259,10 +2950,22 @@
         <v>91</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
@@ -2288,10 +2991,22 @@
         <v>91</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -2319,8 +3034,20 @@
       <c r="I51" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -2346,10 +3073,22 @@
         <v>91</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -2375,10 +3114,22 @@
         <v>92</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2404,10 +3155,22 @@
         <v>91</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -2433,10 +3196,22 @@
         <v>91</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -2464,8 +3239,20 @@
       <c r="I56" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -2493,8 +3280,20 @@
       <c r="I57" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -2522,8 +3321,20 @@
       <c r="I58" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2551,8 +3362,20 @@
       <c r="I59" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2580,8 +3403,20 @@
       <c r="I60" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
@@ -2607,10 +3442,22 @@
         <v>91</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -2638,8 +3485,20 @@
       <c r="I62" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
@@ -2667,8 +3526,20 @@
       <c r="I63" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2696,8 +3567,20 @@
       <c r="I64" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
@@ -2720,13 +3603,25 @@
         <v>92</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>22</v>
       </c>
@@ -2754,8 +3649,20 @@
       <c r="I66" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -2781,10 +3688,22 @@
         <v>91</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>76</v>
       </c>
@@ -2812,8 +3731,20 @@
       <c r="I68" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
@@ -2839,10 +3770,22 @@
         <v>91</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -2870,8 +3813,20 @@
       <c r="I70" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -2899,8 +3854,20 @@
       <c r="I71" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -2926,10 +3893,22 @@
         <v>91</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -2955,10 +3934,22 @@
         <v>91</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>78</v>
       </c>
@@ -2984,10 +3975,22 @@
         <v>91</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
@@ -3015,8 +4018,20 @@
       <c r="I75" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -3042,10 +4057,22 @@
         <v>91</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>78</v>
       </c>
@@ -3071,10 +4098,22 @@
         <v>91</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -3100,10 +4139,22 @@
         <v>91</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3129,10 +4180,22 @@
         <v>91</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -3160,8 +4223,20 @@
       <c r="I80" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -3189,8 +4264,20 @@
       <c r="I81" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -3218,8 +4305,20 @@
       <c r="I82" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -3247,8 +4346,20 @@
       <c r="I83" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>80</v>
       </c>
@@ -3274,10 +4385,22 @@
         <v>91</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>80</v>
       </c>
@@ -3304,6 +4427,18 @@
       </c>
       <c r="I85" s="1" t="s">
         <v>92</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating attribute candidate column
</commit_message>
<xml_diff>
--- a/NorthwindTablesAndColumns.xlsx
+++ b/NorthwindTablesAndColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\YUU-LearnToCode\DataAnalytics\week_9\W9_Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672DEA63-CC2C-48EF-9C6B-06D596721BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96464529-702D-4243-89AC-E3412EF85E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{901F5D27-877F-4C94-89AE-9A9B6ECE5CB6}"/>
   </bookViews>
@@ -930,10 +930,10 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M86" sqref="M86"/>
+      <selection pane="bottomRight" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1029,7 @@
         <v>92</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>92</v>
@@ -1070,7 +1070,7 @@
         <v>91</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>92</v>
@@ -1234,7 +1234,7 @@
         <v>91</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>92</v>
@@ -1275,7 +1275,7 @@
         <v>91</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>92</v>
@@ -1316,7 +1316,7 @@
         <v>92</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>92</v>
@@ -1357,7 +1357,7 @@
         <v>92</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>92</v>
@@ -1685,7 +1685,7 @@
         <v>91</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>92</v>
@@ -1726,7 +1726,7 @@
         <v>91</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>92</v>
@@ -1767,7 +1767,7 @@
         <v>91</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>92</v>
@@ -1808,7 +1808,7 @@
         <v>91</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>92</v>
@@ -1849,7 +1849,7 @@
         <v>91</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>92</v>
@@ -1890,7 +1890,7 @@
         <v>91</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>92</v>
@@ -1972,7 +1972,7 @@
         <v>91</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>92</v>
@@ -2013,7 +2013,7 @@
         <v>91</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>92</v>
@@ -2054,7 +2054,7 @@
         <v>91</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>92</v>
@@ -2095,7 +2095,7 @@
         <v>91</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>92</v>
@@ -2300,7 +2300,7 @@
         <v>92</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>92</v>
@@ -2669,7 +2669,7 @@
         <v>92</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>92</v>
@@ -2710,7 +2710,7 @@
         <v>92</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>92</v>
@@ -2751,7 +2751,7 @@
         <v>92</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>92</v>
@@ -2792,7 +2792,7 @@
         <v>92</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>92</v>
@@ -2833,7 +2833,7 @@
         <v>92</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>92</v>
@@ -2874,7 +2874,7 @@
         <v>92</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>92</v>
@@ -2915,7 +2915,7 @@
         <v>91</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>92</v>
@@ -2956,7 +2956,7 @@
         <v>91</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>126</v>
@@ -3284,7 +3284,7 @@
         <v>91</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>92</v>
@@ -3407,7 +3407,7 @@
         <v>91</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>92</v>
@@ -3489,7 +3489,7 @@
         <v>91</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>92</v>
@@ -3530,7 +3530,7 @@
         <v>91</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>92</v>
@@ -3571,7 +3571,7 @@
         <v>91</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>92</v>
@@ -3612,7 +3612,7 @@
         <v>92</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>92</v>
@@ -3653,7 +3653,7 @@
         <v>92</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>92</v>
@@ -3694,7 +3694,7 @@
         <v>91</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>92</v>
@@ -3735,7 +3735,7 @@
         <v>92</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>92</v>
@@ -3858,7 +3858,7 @@
         <v>92</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>92</v>
@@ -3899,7 +3899,7 @@
         <v>91</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>92</v>
@@ -3940,7 +3940,7 @@
         <v>91</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>92</v>
@@ -3981,7 +3981,7 @@
         <v>91</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>92</v>
@@ -4063,7 +4063,7 @@
         <v>91</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>92</v>
@@ -4104,7 +4104,7 @@
         <v>91</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>92</v>
@@ -4145,7 +4145,7 @@
         <v>91</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>92</v>
@@ -4186,7 +4186,7 @@
         <v>91</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>92</v>
@@ -4350,7 +4350,7 @@
         <v>92</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>92</v>
@@ -4391,7 +4391,7 @@
         <v>91</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>92</v>
@@ -4432,7 +4432,7 @@
         <v>92</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>92</v>
@@ -4456,25 +4456,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA5D0A6329BB324E86983B32928CFC2E" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b28f3bc5995c0091f528145aa367664">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xmlns:ns3="ced60a7f-99b1-48d2-b555-34851c8026ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48800952b0413791e1a5c8543532e00d" ns2:_="" ns3:_="">
     <xsd:import namespace="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
@@ -4715,6 +4696,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ced60a7f-99b1-48d2-b555-34851c8026ae">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="9e0b35a9-e6cb-436b-81d4-4440ba439ca5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0257D61C-6042-483B-9C34-3DE0D82CB154}">
   <ds:schemaRefs>
@@ -4724,17 +4724,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
-    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0F2F57-CFBB-4DE2-9688-0C0C6A435162}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4751,4 +4740,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BB560F9-4CC1-4243-8F16-7FDC2CD703FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ced60a7f-99b1-48d2-b555-34851c8026ae"/>
+    <ds:schemaRef ds:uri="9e0b35a9-e6cb-436b-81d4-4440ba439ca5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>